<commit_message>
Updated to new Board Layout and Schematic
</commit_message>
<xml_diff>
--- a/BOM/BOM.xlsx
+++ b/BOM/BOM.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="109">
   <si>
     <t>BOM</t>
   </si>
@@ -189,9 +189,6 @@
     <t>http://cache.national.com/ds/LM/LM4889.pdf</t>
   </si>
   <si>
-    <t>Capacitor (20%)</t>
-  </si>
-  <si>
     <t>R296-10241-5-ND</t>
   </si>
   <si>
@@ -268,13 +265,105 @@
   </si>
   <si>
     <t>http://ww1.microchip.com/downloads/en/DeviceDoc/S71327_04.pdf</t>
+  </si>
+  <si>
+    <t>470nF Ceramic</t>
+  </si>
+  <si>
+    <t>1uF Ceramic</t>
+  </si>
+  <si>
+    <t>EMK212B7105KG-T</t>
+  </si>
+  <si>
+    <t>Taiyo Yuden</t>
+  </si>
+  <si>
+    <t>587-1283-1-ND</t>
+  </si>
+  <si>
+    <t>EMK212B7474KD-T</t>
+  </si>
+  <si>
+    <t>587-1282-1-ND</t>
+  </si>
+  <si>
+    <t>AVX Corporation</t>
+  </si>
+  <si>
+    <t>CC0805KRX7R9BB104</t>
+  </si>
+  <si>
+    <t>311-1140-1-ND</t>
+  </si>
+  <si>
+    <t>Yageo</t>
+  </si>
+  <si>
+    <t>Min Qty. of 10</t>
+  </si>
+  <si>
+    <t>500R15W103KV4T</t>
+  </si>
+  <si>
+    <t>Johansen Dielectrics Inc</t>
+  </si>
+  <si>
+    <t>709-1188-1-ND</t>
+  </si>
+  <si>
+    <t>08051C332KAT2A</t>
+  </si>
+  <si>
+    <t>478-1355-1-ND</t>
+  </si>
+  <si>
+    <t>10nF Ceramic</t>
+  </si>
+  <si>
+    <t>100nF Ceramic</t>
+  </si>
+  <si>
+    <t>3.3nF Ceramic</t>
+  </si>
+  <si>
+    <t>10 kΩ Potentiometer</t>
+  </si>
+  <si>
+    <r>
+      <t>2.2 k</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Ω Chip Resistor</t>
+    </r>
+  </si>
+  <si>
+    <t>10 kΩ Chip Resistor</t>
+  </si>
+  <si>
+    <t>100 kΩ Chip Resistor</t>
+  </si>
+  <si>
+    <t>100 Ω Chip Resistor</t>
+  </si>
+  <si>
+    <t>20 kΩ Chip Resistor</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="169" formatCode="0.000"/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -297,6 +386,12 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -318,7 +413,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -500,15 +595,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -517,7 +603,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -591,10 +677,31 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -899,10 +1006,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K18"/>
+  <dimension ref="A1:K30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J25" sqref="J25"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -956,10 +1063,10 @@
         <v>7</v>
       </c>
       <c r="H3" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="I3" s="18" t="s">
         <v>79</v>
-      </c>
-      <c r="I3" s="18" t="s">
-        <v>80</v>
       </c>
       <c r="J3" s="18" t="s">
         <v>8</v>
@@ -982,7 +1089,7 @@
         <v>47</v>
       </c>
       <c r="E4" s="21" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F4" s="21">
         <v>1</v>
@@ -993,8 +1100,8 @@
       <c r="H4" s="22">
         <v>4.4000000000000004</v>
       </c>
-      <c r="I4" s="22">
-        <f>H4*F4</f>
+      <c r="I4" s="29">
+        <f t="shared" ref="I4:I21" si="0">H4*F4</f>
         <v>4.4000000000000004</v>
       </c>
       <c r="J4" s="21" t="s">
@@ -1029,8 +1136,8 @@
       <c r="H5" s="3">
         <v>1.66</v>
       </c>
-      <c r="I5" s="7">
-        <f>H5*F5</f>
+      <c r="I5" s="30">
+        <f t="shared" si="0"/>
         <v>1.66</v>
       </c>
       <c r="J5" s="2" t="s">
@@ -1065,8 +1172,8 @@
       <c r="H6" s="3">
         <v>2.8</v>
       </c>
-      <c r="I6" s="7">
-        <f>H6*F6</f>
+      <c r="I6" s="30">
+        <f t="shared" si="0"/>
         <v>2.8</v>
       </c>
       <c r="J6" s="2" t="s">
@@ -1101,15 +1208,15 @@
       <c r="H7" s="2">
         <v>2.5499999999999998</v>
       </c>
-      <c r="I7" s="7">
-        <f>H7*F7</f>
+      <c r="I7" s="30">
+        <f t="shared" si="0"/>
         <v>2.5499999999999998</v>
       </c>
       <c r="J7" s="2" t="s">
         <v>11</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="8" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -1137,8 +1244,8 @@
       <c r="H8" s="7">
         <v>1.57</v>
       </c>
-      <c r="I8" s="7">
-        <f>H8*F8</f>
+      <c r="I8" s="30">
+        <f t="shared" si="0"/>
         <v>1.57</v>
       </c>
       <c r="J8" s="6" t="s">
@@ -1173,8 +1280,8 @@
       <c r="H9" s="6">
         <v>1.22</v>
       </c>
-      <c r="I9" s="7">
-        <f>H9*F9</f>
+      <c r="I9" s="30">
+        <f t="shared" si="0"/>
         <v>1.22</v>
       </c>
       <c r="J9" s="6" t="s">
@@ -1209,8 +1316,8 @@
       <c r="H10" s="7">
         <v>1.04</v>
       </c>
-      <c r="I10" s="7">
-        <f>H10*F10</f>
+      <c r="I10" s="30">
+        <f t="shared" si="0"/>
         <v>1.04</v>
       </c>
       <c r="J10" s="6" t="s">
@@ -1222,38 +1329,38 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B11" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="B11" s="12" t="s">
+      <c r="C11" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="C11" s="12" t="s">
-        <v>61</v>
-      </c>
       <c r="D11" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="E11" s="12" t="s">
         <v>60</v>
-      </c>
-      <c r="E11" s="12" t="s">
-        <v>61</v>
       </c>
       <c r="F11" s="12">
         <v>1</v>
       </c>
       <c r="G11" s="12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H11" s="12">
         <v>1.5</v>
       </c>
-      <c r="I11" s="7">
-        <f>H11*F11</f>
+      <c r="I11" s="30">
+        <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
       <c r="J11" s="12" t="s">
         <v>11</v>
       </c>
       <c r="K11" s="14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -1281,8 +1388,8 @@
       <c r="H12" s="13">
         <v>0.45</v>
       </c>
-      <c r="I12" s="13">
-        <f>H12*F12</f>
+      <c r="I12" s="31">
+        <f t="shared" si="0"/>
         <v>0.45</v>
       </c>
       <c r="J12" s="12" t="s">
@@ -1293,71 +1400,71 @@
       </c>
     </row>
     <row r="13" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D13" s="6" t="s">
+      <c r="A13" s="27" t="s">
+        <v>83</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="D13" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="E13" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F13" s="6">
-        <v>15</v>
-      </c>
-      <c r="G13" s="10" t="s">
+      <c r="E13" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="F13" s="12">
+        <v>1</v>
+      </c>
+      <c r="G13" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="H13" s="7">
-        <v>0.2</v>
-      </c>
-      <c r="I13" s="7">
-        <f>H13*F13</f>
-        <v>3</v>
-      </c>
-      <c r="J13" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="K13" s="8" t="s">
+      <c r="H13" s="12">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="I13" s="31">
+        <f>F13*H13</f>
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="J13" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="K13" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D14" s="6" t="s">
+      <c r="A14" s="27" t="s">
+        <v>84</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="D14" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="E14" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F14" s="6">
-        <v>15</v>
-      </c>
-      <c r="G14" s="10" t="s">
+      <c r="E14" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="F14" s="12">
+        <v>4</v>
+      </c>
+      <c r="G14" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="H14" s="7">
-        <v>0.04</v>
-      </c>
-      <c r="I14" s="7">
-        <f>H14*F14</f>
-        <v>0.6</v>
-      </c>
-      <c r="J14" s="6" t="s">
+      <c r="H14" s="12">
+        <v>0.24</v>
+      </c>
+      <c r="I14" s="31">
+        <f>F14*H14</f>
+        <v>0.96</v>
+      </c>
+      <c r="J14" s="12" t="s">
         <v>11</v>
       </c>
       <c r="K14" s="15" t="s">
@@ -1365,126 +1472,324 @@
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
-        <v>63</v>
+      <c r="A15" s="27" t="s">
+        <v>100</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>66</v>
+        <v>96</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>65</v>
+        <v>95</v>
       </c>
       <c r="D15" s="12" t="s">
         <v>47</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>64</v>
+        <v>97</v>
       </c>
       <c r="F15" s="12">
-        <v>2</v>
-      </c>
-      <c r="G15" s="12" t="s">
-        <v>67</v>
+        <v>8</v>
+      </c>
+      <c r="G15" s="26" t="s">
+        <v>52</v>
       </c>
       <c r="H15" s="12">
-        <v>0.35</v>
-      </c>
-      <c r="I15" s="12">
-        <f>H15*F15</f>
-        <v>0.7</v>
+        <v>4.3999999999999997E-2</v>
+      </c>
+      <c r="I15" s="31">
+        <f>F15*H15</f>
+        <v>0.35199999999999998</v>
       </c>
       <c r="J15" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="K15" s="14" t="s">
-        <v>73</v>
+        <v>94</v>
+      </c>
+      <c r="K15" s="28" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="5" t="s">
-        <v>68</v>
+      <c r="A16" s="27" t="s">
+        <v>101</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>69</v>
+        <v>93</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>70</v>
+        <v>91</v>
       </c>
       <c r="D16" s="12" t="s">
         <v>47</v>
       </c>
       <c r="E16" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="F16" s="12">
+        <v>8</v>
+      </c>
+      <c r="G16" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="H16" s="12">
+        <v>6.3E-2</v>
+      </c>
+      <c r="I16" s="31">
+        <f>F16*H16</f>
+        <v>0.504</v>
+      </c>
+      <c r="J16" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="K16" s="28" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="27" t="s">
+        <v>102</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="D17" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="E17" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="F17" s="12">
+        <v>3</v>
+      </c>
+      <c r="G17" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="H17" s="12">
+        <v>0.24</v>
+      </c>
+      <c r="I17" s="31">
+        <f>F17*H17</f>
+        <v>0.72</v>
+      </c>
+      <c r="J17" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="K17" s="28" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F18" s="6">
+        <v>15</v>
+      </c>
+      <c r="G18" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="H18" s="7">
+        <v>0.04</v>
+      </c>
+      <c r="I18" s="30">
+        <f t="shared" si="0"/>
+        <v>0.6</v>
+      </c>
+      <c r="J18" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="K18" s="28" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B19" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="D19" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="E19" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="F19" s="12">
+        <v>2</v>
+      </c>
+      <c r="G19" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="H19" s="12">
+        <v>0.35</v>
+      </c>
+      <c r="I19" s="31">
+        <f t="shared" si="0"/>
+        <v>0.7</v>
+      </c>
+      <c r="J19" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="K19" s="14" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="D20" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="E20" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="F20" s="12">
+        <v>1</v>
+      </c>
+      <c r="G20" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="F16" s="12">
+      <c r="H20" s="12">
+        <v>0.52</v>
+      </c>
+      <c r="I20" s="31">
+        <f t="shared" si="0"/>
+        <v>0.52</v>
+      </c>
+      <c r="J20" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="K20" s="14" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="B21" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="C21" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="D21" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="E21" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="F21" s="16">
+        <v>3</v>
+      </c>
+      <c r="G21" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="H21" s="16">
+        <v>0.44</v>
+      </c>
+      <c r="I21" s="32">
+        <f t="shared" si="0"/>
+        <v>1.32</v>
+      </c>
+      <c r="J21" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="K21" s="24" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G22" s="25" t="s">
+        <v>81</v>
+      </c>
+      <c r="H22" s="25"/>
+      <c r="I22" s="33">
+        <f>SUM(I5:I21)</f>
+        <v>18.745999999999999</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="F24" s="1">
         <v>1</v>
       </c>
-      <c r="G16" s="12" t="s">
-        <v>72</v>
-      </c>
-      <c r="H16" s="12">
-        <v>0.52</v>
-      </c>
-      <c r="I16" s="12">
-        <f>H16*F16</f>
-        <v>0.52</v>
-      </c>
-      <c r="J16" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="K16" s="14" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="B17" s="16" t="s">
-        <v>76</v>
-      </c>
-      <c r="C17" s="16" t="s">
-        <v>77</v>
-      </c>
-      <c r="D17" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="E17" s="16" t="s">
-        <v>78</v>
-      </c>
-      <c r="F17" s="16">
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="F25" s="1">
         <v>3</v>
       </c>
-      <c r="G17" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="H17" s="16">
-        <v>0.44</v>
-      </c>
-      <c r="I17" s="16">
-        <f>H17*F17</f>
-        <v>1.32</v>
-      </c>
-      <c r="J17" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="K17" s="24" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="G18" s="25" t="s">
-        <v>82</v>
-      </c>
-      <c r="H18" s="25"/>
-      <c r="I18" s="26">
-        <f>SUM(I5:I17)</f>
-        <v>18.93</v>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="F26" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="F27" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="F28" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="F29" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F30" s="1">
+        <f>SUM(F24:F29)</f>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="G22:H22"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="K5" r:id="rId1"/>
@@ -1492,15 +1797,15 @@
     <hyperlink ref="K8" r:id="rId3"/>
     <hyperlink ref="K4" r:id="rId4"/>
     <hyperlink ref="K10" r:id="rId5"/>
-    <hyperlink ref="K16" r:id="rId6"/>
-    <hyperlink ref="K15" r:id="rId7"/>
+    <hyperlink ref="K20" r:id="rId6"/>
+    <hyperlink ref="K19" r:id="rId7"/>
     <hyperlink ref="K11" r:id="rId8"/>
-    <hyperlink ref="K17" r:id="rId9"/>
+    <hyperlink ref="K21" r:id="rId9"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" horizontalDpi="4294967293" verticalDpi="300" r:id="rId10"/>
   <ignoredErrors>
-    <ignoredError sqref="G13:G14" numberStoredAsText="1"/>
+    <ignoredError sqref="G17:G18 G13:G16" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Final Board Layout and Files
</commit_message>
<xml_diff>
--- a/BOM/BOM.xlsx
+++ b/BOM/BOM.xlsx
@@ -361,7 +361,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -603,7 +603,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -641,9 +641,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
@@ -662,46 +659,61 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1009,7 +1021,7 @@
   <dimension ref="A1:K30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1041,73 +1053,73 @@
     </row>
     <row r="2" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="18" t="s">
+      <c r="C3" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="18" t="s">
+      <c r="D3" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="18" t="s">
+      <c r="E3" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="18" t="s">
+      <c r="F3" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="18" t="s">
+      <c r="G3" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="18" t="s">
+      <c r="H3" s="17" t="s">
         <v>78</v>
       </c>
-      <c r="I3" s="18" t="s">
+      <c r="I3" s="17" t="s">
         <v>79</v>
       </c>
-      <c r="J3" s="18" t="s">
+      <c r="J3" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="K3" s="19" t="s">
+      <c r="K3" s="18" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="21" t="s">
+      <c r="B4" s="34" t="s">
         <v>29</v>
       </c>
-      <c r="C4" s="21" t="s">
+      <c r="C4" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="21" t="s">
+      <c r="D4" s="34" t="s">
         <v>47</v>
       </c>
-      <c r="E4" s="21" t="s">
+      <c r="E4" s="34" t="s">
         <v>57</v>
       </c>
-      <c r="F4" s="21">
+      <c r="F4" s="34">
         <v>1</v>
       </c>
-      <c r="G4" s="21" t="s">
+      <c r="G4" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="22">
+      <c r="H4" s="35">
         <v>4.4000000000000004</v>
       </c>
-      <c r="I4" s="29">
+      <c r="I4" s="36">
         <f t="shared" ref="I4:I21" si="0">H4*F4</f>
         <v>4.4000000000000004</v>
       </c>
-      <c r="J4" s="21" t="s">
+      <c r="J4" s="34" t="s">
         <v>46</v>
       </c>
-      <c r="K4" s="23" t="s">
+      <c r="K4" s="37" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1136,7 +1148,7 @@
       <c r="H5" s="3">
         <v>1.66</v>
       </c>
-      <c r="I5" s="30">
+      <c r="I5" s="23">
         <f t="shared" si="0"/>
         <v>1.66</v>
       </c>
@@ -1172,7 +1184,7 @@
       <c r="H6" s="3">
         <v>2.8</v>
       </c>
-      <c r="I6" s="30">
+      <c r="I6" s="23">
         <f t="shared" si="0"/>
         <v>2.8</v>
       </c>
@@ -1208,7 +1220,7 @@
       <c r="H7" s="2">
         <v>2.5499999999999998</v>
       </c>
-      <c r="I7" s="30">
+      <c r="I7" s="23">
         <f t="shared" si="0"/>
         <v>2.5499999999999998</v>
       </c>
@@ -1244,7 +1256,7 @@
       <c r="H8" s="7">
         <v>1.57</v>
       </c>
-      <c r="I8" s="30">
+      <c r="I8" s="23">
         <f t="shared" si="0"/>
         <v>1.57</v>
       </c>
@@ -1280,7 +1292,7 @@
       <c r="H9" s="6">
         <v>1.22</v>
       </c>
-      <c r="I9" s="30">
+      <c r="I9" s="23">
         <f t="shared" si="0"/>
         <v>1.22</v>
       </c>
@@ -1316,7 +1328,7 @@
       <c r="H10" s="7">
         <v>1.04</v>
       </c>
-      <c r="I10" s="30">
+      <c r="I10" s="23">
         <f t="shared" si="0"/>
         <v>1.04</v>
       </c>
@@ -1352,55 +1364,55 @@
       <c r="H11" s="12">
         <v>1.5</v>
       </c>
-      <c r="I11" s="30">
+      <c r="I11" s="23">
         <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
       <c r="J11" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="K11" s="14" t="s">
+      <c r="K11" s="13" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="B12" s="12" t="s">
+      <c r="B12" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="C12" s="12" t="s">
+      <c r="C12" s="29" t="s">
         <v>48</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D12" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="E12" s="12" t="s">
+      <c r="E12" s="29" t="s">
         <v>49</v>
       </c>
-      <c r="F12" s="12">
+      <c r="F12" s="29">
         <v>1</v>
       </c>
-      <c r="G12" s="12" t="s">
+      <c r="G12" s="29" t="s">
         <v>50</v>
       </c>
-      <c r="H12" s="13">
+      <c r="H12" s="30">
         <v>0.45</v>
       </c>
       <c r="I12" s="31">
         <f t="shared" si="0"/>
         <v>0.45</v>
       </c>
-      <c r="J12" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="K12" s="14" t="s">
+      <c r="J12" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="K12" s="32" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="27" t="s">
+      <c r="A13" s="21" t="s">
         <v>83</v>
       </c>
       <c r="B13" s="12" t="s">
@@ -1418,13 +1430,13 @@
       <c r="F13" s="12">
         <v>1</v>
       </c>
-      <c r="G13" s="26" t="s">
+      <c r="G13" s="20" t="s">
         <v>52</v>
       </c>
       <c r="H13" s="12">
         <v>0.28000000000000003</v>
       </c>
-      <c r="I13" s="31">
+      <c r="I13" s="24">
         <f>F13*H13</f>
         <v>0.28000000000000003</v>
       </c>
@@ -1436,7 +1448,7 @@
       </c>
     </row>
     <row r="14" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="27" t="s">
+      <c r="A14" s="21" t="s">
         <v>84</v>
       </c>
       <c r="B14" s="12" t="s">
@@ -1454,25 +1466,25 @@
       <c r="F14" s="12">
         <v>4</v>
       </c>
-      <c r="G14" s="26" t="s">
+      <c r="G14" s="20" t="s">
         <v>52</v>
       </c>
       <c r="H14" s="12">
         <v>0.24</v>
       </c>
-      <c r="I14" s="31">
+      <c r="I14" s="24">
         <f>F14*H14</f>
         <v>0.96</v>
       </c>
       <c r="J14" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="K14" s="15" t="s">
+      <c r="K14" s="14" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="27" t="s">
+      <c r="A15" s="21" t="s">
         <v>100</v>
       </c>
       <c r="B15" s="12" t="s">
@@ -1490,25 +1502,25 @@
       <c r="F15" s="12">
         <v>8</v>
       </c>
-      <c r="G15" s="26" t="s">
+      <c r="G15" s="20" t="s">
         <v>52</v>
       </c>
       <c r="H15" s="12">
         <v>4.3999999999999997E-2</v>
       </c>
-      <c r="I15" s="31">
+      <c r="I15" s="24">
         <f>F15*H15</f>
         <v>0.35199999999999998</v>
       </c>
       <c r="J15" s="12" t="s">
         <v>94</v>
       </c>
-      <c r="K15" s="28" t="s">
+      <c r="K15" s="22" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="27" t="s">
+      <c r="A16" s="21" t="s">
         <v>101</v>
       </c>
       <c r="B16" s="12" t="s">
@@ -1526,25 +1538,25 @@
       <c r="F16" s="12">
         <v>8</v>
       </c>
-      <c r="G16" s="26" t="s">
+      <c r="G16" s="20" t="s">
         <v>52</v>
       </c>
       <c r="H16" s="12">
         <v>6.3E-2</v>
       </c>
-      <c r="I16" s="31">
+      <c r="I16" s="24">
         <f>F16*H16</f>
         <v>0.504</v>
       </c>
       <c r="J16" s="12" t="s">
         <v>94</v>
       </c>
-      <c r="K16" s="28" t="s">
+      <c r="K16" s="22" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="27" t="s">
+      <c r="A17" s="21" t="s">
         <v>102</v>
       </c>
       <c r="B17" s="12" t="s">
@@ -1562,20 +1574,20 @@
       <c r="F17" s="12">
         <v>3</v>
       </c>
-      <c r="G17" s="26" t="s">
+      <c r="G17" s="20" t="s">
         <v>52</v>
       </c>
       <c r="H17" s="12">
         <v>0.24</v>
       </c>
-      <c r="I17" s="31">
+      <c r="I17" s="24">
         <f>F17*H17</f>
         <v>0.72</v>
       </c>
       <c r="J17" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="K17" s="28" t="s">
+      <c r="K17" s="22" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1604,14 +1616,14 @@
       <c r="H18" s="7">
         <v>0.04</v>
       </c>
-      <c r="I18" s="30">
+      <c r="I18" s="23">
         <f t="shared" si="0"/>
         <v>0.6</v>
       </c>
       <c r="J18" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="K18" s="28" t="s">
+      <c r="K18" s="22" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1640,14 +1652,14 @@
       <c r="H19" s="12">
         <v>0.35</v>
       </c>
-      <c r="I19" s="31">
+      <c r="I19" s="24">
         <f t="shared" si="0"/>
         <v>0.7</v>
       </c>
       <c r="J19" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="K19" s="14" t="s">
+      <c r="K19" s="13" t="s">
         <v>72</v>
       </c>
     </row>
@@ -1676,14 +1688,14 @@
       <c r="H20" s="12">
         <v>0.52</v>
       </c>
-      <c r="I20" s="31">
+      <c r="I20" s="24">
         <f t="shared" si="0"/>
         <v>0.52</v>
       </c>
       <c r="J20" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="K20" s="14" t="s">
+      <c r="K20" s="13" t="s">
         <v>67</v>
       </c>
     </row>
@@ -1691,46 +1703,46 @@
       <c r="A21" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="B21" s="16" t="s">
+      <c r="B21" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="C21" s="16" t="s">
+      <c r="C21" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="D21" s="16" t="s">
+      <c r="D21" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="E21" s="16" t="s">
+      <c r="E21" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="F21" s="16">
+      <c r="F21" s="15">
         <v>3</v>
       </c>
-      <c r="G21" s="16" t="s">
+      <c r="G21" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="H21" s="16">
+      <c r="H21" s="15">
         <v>0.44</v>
       </c>
-      <c r="I21" s="32">
+      <c r="I21" s="25">
         <f t="shared" si="0"/>
         <v>1.32</v>
       </c>
-      <c r="J21" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="K21" s="24" t="s">
+      <c r="J21" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="K21" s="19" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="G22" s="25" t="s">
+      <c r="G22" s="27" t="s">
         <v>81</v>
       </c>
-      <c r="H22" s="25"/>
-      <c r="I22" s="33">
-        <f>SUM(I5:I21)</f>
-        <v>18.745999999999999</v>
+      <c r="H22" s="27"/>
+      <c r="I22" s="26">
+        <f>SUM(I4:I11)+SUM(I13:I21)</f>
+        <v>22.696000000000002</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Adding new Board Layout Files and Updated BOM
</commit_message>
<xml_diff>
--- a/BOM/BOM.xlsx
+++ b/BOM/BOM.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="122">
   <si>
     <t>BOM</t>
   </si>
@@ -48,9 +48,6 @@
     <t>Datasheet</t>
   </si>
   <si>
-    <t>8-DIP</t>
-  </si>
-  <si>
     <t>-</t>
   </si>
   <si>
@@ -99,18 +96,12 @@
     <t>Rail-to-Rail Op-Amp</t>
   </si>
   <si>
-    <t>Resistors (5%)</t>
-  </si>
-  <si>
     <t>http://www.ti.com/lit/ds/symlink/tlc2201.pdf</t>
   </si>
   <si>
     <t>Texas Instruments</t>
   </si>
   <si>
-    <t>TLC2201CP</t>
-  </si>
-  <si>
     <t>CUI Inc.</t>
   </si>
   <si>
@@ -156,9 +147,6 @@
     <t>SST25VF032B-80-4I-S2AF-ND</t>
   </si>
   <si>
-    <t>Need Cheaper! And SMD</t>
-  </si>
-  <si>
     <t>Digi-Key</t>
   </si>
   <si>
@@ -187,9 +175,6 @@
   </si>
   <si>
     <t>http://cache.national.com/ds/LM/LM4889.pdf</t>
-  </si>
-  <si>
-    <t>R296-10241-5-ND</t>
   </si>
   <si>
     <t>Pin Connectors</t>
@@ -354,6 +339,60 @@
   </si>
   <si>
     <t>20 kΩ Chip Resistor</t>
+  </si>
+  <si>
+    <t>Stackpole Electronics</t>
+  </si>
+  <si>
+    <t>RMCF0805JT2K20</t>
+  </si>
+  <si>
+    <t>RMCF0805JT2K20CT-ND</t>
+  </si>
+  <si>
+    <t>http://www.seielect.com/Catalog/SEI-RMCF.pdf</t>
+  </si>
+  <si>
+    <t>RMCF0805JT10K0</t>
+  </si>
+  <si>
+    <t>RMCF0805JT10K0CT-ND</t>
+  </si>
+  <si>
+    <t>RMCF0805JT100K</t>
+  </si>
+  <si>
+    <t>RMCF0805JT100KCT-ND</t>
+  </si>
+  <si>
+    <t>RMCF0805JT100R</t>
+  </si>
+  <si>
+    <t>RMCF0805JT100RCT-ND</t>
+  </si>
+  <si>
+    <t>RMCF0805JT20K0</t>
+  </si>
+  <si>
+    <t>RMCF0805JT20K0CT-ND</t>
+  </si>
+  <si>
+    <t>Bourns Inc.</t>
+  </si>
+  <si>
+    <t>3352T-1-103LF</t>
+  </si>
+  <si>
+    <t>3352T-103LF-ND</t>
+  </si>
+  <si>
+    <t>http://www.bourns.com/data/global/PDFs/3352.pdf</t>
+  </si>
+  <si>
+    <t>TLC2201CD</t>
+  </si>
+  <si>
+    <t>296-2425-5-ND</t>
   </si>
 </sst>
 </file>
@@ -603,7 +642,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -632,12 +671,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -647,9 +680,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -659,9 +689,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -677,43 +704,40 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1018,10 +1042,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K30"/>
+  <dimension ref="A1:K27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+      <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1032,7 +1056,7 @@
     <col min="4" max="4" width="9.5703125" style="1" customWidth="1"/>
     <col min="5" max="5" width="27.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="4.7109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" style="1" customWidth="1"/>
     <col min="8" max="8" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="23.85546875" style="1" customWidth="1"/>
@@ -1053,755 +1077,881 @@
     </row>
     <row r="2" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="C3" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="17" t="s">
+      <c r="D3" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="17" t="s">
+      <c r="E3" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="17" t="s">
+      <c r="F3" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="17" t="s">
+      <c r="G3" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="17" t="s">
-        <v>78</v>
-      </c>
-      <c r="I3" s="17" t="s">
-        <v>79</v>
-      </c>
-      <c r="J3" s="17" t="s">
+      <c r="H3" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="I3" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="J3" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="K3" s="18" t="s">
+      <c r="K3" s="15" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="33" t="s">
+      <c r="A4" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="23" t="s">
+        <v>120</v>
+      </c>
+      <c r="D4" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="E4" s="23" t="s">
+        <v>121</v>
+      </c>
+      <c r="F4" s="23">
+        <v>1</v>
+      </c>
+      <c r="G4" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="H4" s="24">
+        <v>5.32</v>
+      </c>
+      <c r="I4" s="25">
+        <f t="shared" ref="I4:I25" si="0">H4*F4</f>
+        <v>5.32</v>
+      </c>
+      <c r="J4" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="K4" s="26" t="s">
         <v>26</v>
-      </c>
-      <c r="B4" s="34" t="s">
-        <v>29</v>
-      </c>
-      <c r="C4" s="34" t="s">
-        <v>30</v>
-      </c>
-      <c r="D4" s="34" t="s">
-        <v>47</v>
-      </c>
-      <c r="E4" s="34" t="s">
-        <v>57</v>
-      </c>
-      <c r="F4" s="34">
-        <v>1</v>
-      </c>
-      <c r="G4" s="34" t="s">
-        <v>10</v>
-      </c>
-      <c r="H4" s="35">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="I4" s="36">
-        <f t="shared" ref="I4:I21" si="0">H4*F4</f>
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="J4" s="34" t="s">
-        <v>46</v>
-      </c>
-      <c r="K4" s="37" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F5" s="2">
         <v>1</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="H5" s="3">
         <v>1.66</v>
       </c>
-      <c r="I5" s="23">
+      <c r="I5" s="19">
         <f t="shared" si="0"/>
         <v>1.66</v>
       </c>
       <c r="J5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="K5" s="4" t="s">
         <v>11</v>
-      </c>
-      <c r="K5" s="4" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="D6" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>17</v>
       </c>
       <c r="F6" s="2">
         <v>1</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H6" s="3">
         <v>2.8</v>
       </c>
-      <c r="I6" s="23">
+      <c r="I6" s="19">
         <f t="shared" si="0"/>
         <v>2.8</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="F7" s="2">
         <v>1</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H7" s="2">
         <v>2.5499999999999998</v>
       </c>
-      <c r="I7" s="23">
+      <c r="I7" s="19">
         <f t="shared" si="0"/>
         <v>2.5499999999999998</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="8" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B8" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="D8" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E8" s="6" t="s">
         <v>22</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>23</v>
       </c>
       <c r="F8" s="6">
         <v>1</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="H8" s="7">
         <v>1.57</v>
       </c>
-      <c r="I8" s="23">
+      <c r="I8" s="19">
         <f t="shared" si="0"/>
         <v>1.57</v>
       </c>
       <c r="J8" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K8" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="F9" s="6">
         <v>1</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="H9" s="6">
         <v>1.22</v>
       </c>
-      <c r="I9" s="23">
+      <c r="I9" s="19">
         <f t="shared" si="0"/>
         <v>1.22</v>
       </c>
       <c r="J9" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K9" s="8" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="F10" s="6">
         <v>1</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="H10" s="7">
         <v>1.04</v>
       </c>
-      <c r="I10" s="23">
+      <c r="I10" s="19">
         <f t="shared" si="0"/>
         <v>1.04</v>
       </c>
       <c r="J10" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K10" s="8" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="B11" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="C11" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="D11" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="E11" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="F11" s="12">
+        <v>53</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="F11" s="10">
         <v>1</v>
       </c>
-      <c r="G11" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="H11" s="12">
+      <c r="G11" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="H11" s="10">
         <v>1.5</v>
       </c>
-      <c r="I11" s="23">
+      <c r="I11" s="19">
         <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
-      <c r="J11" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="K11" s="13" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="28" t="s">
-        <v>26</v>
-      </c>
-      <c r="B12" s="29" t="s">
-        <v>36</v>
-      </c>
-      <c r="C12" s="29" t="s">
+      <c r="J11" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="K11" s="11" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="F12" s="10">
+        <v>1</v>
+      </c>
+      <c r="G12" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="D12" s="29" t="s">
-        <v>47</v>
-      </c>
-      <c r="E12" s="29" t="s">
-        <v>49</v>
-      </c>
-      <c r="F12" s="29">
-        <v>1</v>
-      </c>
-      <c r="G12" s="29" t="s">
-        <v>50</v>
-      </c>
-      <c r="H12" s="30">
-        <v>0.45</v>
-      </c>
-      <c r="I12" s="31">
+      <c r="H12" s="10">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="I12" s="20">
+        <f>F12*H12</f>
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="J12" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="K12" s="18" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="F13" s="10">
+        <v>4</v>
+      </c>
+      <c r="G13" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="H13" s="10">
+        <v>0.24</v>
+      </c>
+      <c r="I13" s="20">
+        <f>F13*H13</f>
+        <v>0.96</v>
+      </c>
+      <c r="J13" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="K13" s="12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="F14" s="10">
+        <v>8</v>
+      </c>
+      <c r="G14" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="H14" s="10">
+        <v>4.3999999999999997E-2</v>
+      </c>
+      <c r="I14" s="20">
+        <f>F14*H14</f>
+        <v>0.35199999999999998</v>
+      </c>
+      <c r="J14" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="K14" s="18" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="E15" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="F15" s="10">
+        <v>8</v>
+      </c>
+      <c r="G15" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="H15" s="10">
+        <v>6.3E-2</v>
+      </c>
+      <c r="I15" s="20">
+        <f>F15*H15</f>
+        <v>0.504</v>
+      </c>
+      <c r="J15" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="K15" s="18" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="F16" s="10">
+        <v>3</v>
+      </c>
+      <c r="G16" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="H16" s="10">
+        <v>0.24</v>
+      </c>
+      <c r="I16" s="20">
+        <f>F16*H16</f>
+        <v>0.72</v>
+      </c>
+      <c r="J16" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="K16" s="18" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="E17" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="F17" s="10">
+        <v>2</v>
+      </c>
+      <c r="G17" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="H17" s="10">
+        <v>0.35</v>
+      </c>
+      <c r="I17" s="20">
         <f t="shared" si="0"/>
-        <v>0.45</v>
-      </c>
-      <c r="J12" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="K12" s="32" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="21" t="s">
-        <v>83</v>
-      </c>
-      <c r="B13" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="C13" s="12" t="s">
-        <v>88</v>
-      </c>
-      <c r="D13" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="E13" s="12" t="s">
-        <v>89</v>
-      </c>
-      <c r="F13" s="12">
-        <v>1</v>
-      </c>
-      <c r="G13" s="20" t="s">
-        <v>52</v>
-      </c>
-      <c r="H13" s="12">
-        <v>0.28000000000000003</v>
-      </c>
-      <c r="I13" s="24">
-        <f>F13*H13</f>
-        <v>0.28000000000000003</v>
-      </c>
-      <c r="J13" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="K13" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="21" t="s">
-        <v>84</v>
-      </c>
-      <c r="B14" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="C14" s="12" t="s">
-        <v>85</v>
-      </c>
-      <c r="D14" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="E14" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="F14" s="12">
-        <v>4</v>
-      </c>
-      <c r="G14" s="20" t="s">
-        <v>52</v>
-      </c>
-      <c r="H14" s="12">
-        <v>0.24</v>
-      </c>
-      <c r="I14" s="24">
-        <f>F14*H14</f>
-        <v>0.96</v>
-      </c>
-      <c r="J14" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="K14" s="14" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="21" t="s">
-        <v>100</v>
-      </c>
-      <c r="B15" s="12" t="s">
-        <v>96</v>
-      </c>
-      <c r="C15" s="12" t="s">
-        <v>95</v>
-      </c>
-      <c r="D15" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="E15" s="12" t="s">
-        <v>97</v>
-      </c>
-      <c r="F15" s="12">
-        <v>8</v>
-      </c>
-      <c r="G15" s="20" t="s">
-        <v>52</v>
-      </c>
-      <c r="H15" s="12">
-        <v>4.3999999999999997E-2</v>
-      </c>
-      <c r="I15" s="24">
-        <f>F15*H15</f>
-        <v>0.35199999999999998</v>
-      </c>
-      <c r="J15" s="12" t="s">
-        <v>94</v>
-      </c>
-      <c r="K15" s="22" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="21" t="s">
-        <v>101</v>
-      </c>
-      <c r="B16" s="12" t="s">
-        <v>93</v>
-      </c>
-      <c r="C16" s="12" t="s">
-        <v>91</v>
-      </c>
-      <c r="D16" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="E16" s="12" t="s">
-        <v>92</v>
-      </c>
-      <c r="F16" s="12">
-        <v>8</v>
-      </c>
-      <c r="G16" s="20" t="s">
-        <v>52</v>
-      </c>
-      <c r="H16" s="12">
-        <v>6.3E-2</v>
-      </c>
-      <c r="I16" s="24">
-        <f>F16*H16</f>
-        <v>0.504</v>
-      </c>
-      <c r="J16" s="12" t="s">
-        <v>94</v>
-      </c>
-      <c r="K16" s="22" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="21" t="s">
-        <v>102</v>
-      </c>
-      <c r="B17" s="12" t="s">
-        <v>90</v>
-      </c>
-      <c r="C17" s="12" t="s">
-        <v>98</v>
-      </c>
-      <c r="D17" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="E17" s="12" t="s">
-        <v>99</v>
-      </c>
-      <c r="F17" s="12">
-        <v>3</v>
-      </c>
-      <c r="G17" s="20" t="s">
-        <v>52</v>
-      </c>
-      <c r="H17" s="12">
-        <v>0.24</v>
-      </c>
-      <c r="I17" s="24">
-        <f>F17*H17</f>
-        <v>0.72</v>
-      </c>
-      <c r="J17" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="K17" s="22" t="s">
-        <v>11</v>
+        <v>0.7</v>
+      </c>
+      <c r="J17" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="K17" s="11" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D18" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="E18" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F18" s="6">
-        <v>15</v>
+        <v>62</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="E18" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="F18" s="10">
+        <v>1</v>
       </c>
       <c r="G18" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="H18" s="7">
-        <v>0.04</v>
-      </c>
-      <c r="I18" s="23">
+        <v>66</v>
+      </c>
+      <c r="H18" s="10">
+        <v>0.52</v>
+      </c>
+      <c r="I18" s="20">
         <f t="shared" si="0"/>
-        <v>0.6</v>
-      </c>
-      <c r="J18" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="K18" s="22" t="s">
-        <v>11</v>
+        <v>0.52</v>
+      </c>
+      <c r="J18" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="K18" s="11" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="B19" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="C19" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="D19" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="E19" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="F19" s="12">
-        <v>2</v>
-      </c>
-      <c r="G19" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="H19" s="12">
-        <v>0.35</v>
-      </c>
-      <c r="I19" s="24">
-        <f t="shared" si="0"/>
-        <v>0.7</v>
-      </c>
-      <c r="J19" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="K19" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="E19" s="10" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="B20" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="C20" s="12" t="s">
-        <v>69</v>
-      </c>
-      <c r="D20" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="E20" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="F20" s="12">
-        <v>1</v>
-      </c>
-      <c r="G20" s="12" t="s">
-        <v>71</v>
-      </c>
-      <c r="H20" s="12">
-        <v>0.52</v>
-      </c>
-      <c r="I20" s="24">
-        <f t="shared" si="0"/>
-        <v>0.52</v>
-      </c>
-      <c r="J20" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="K20" s="13" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="B21" s="15" t="s">
-        <v>75</v>
-      </c>
-      <c r="C21" s="15" t="s">
-        <v>76</v>
-      </c>
-      <c r="D21" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="E21" s="15" t="s">
-        <v>77</v>
-      </c>
-      <c r="F21" s="15">
+      <c r="F19" s="10">
         <v>3</v>
       </c>
-      <c r="G21" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="H21" s="15">
+      <c r="G19" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="H19" s="10">
         <v>0.44</v>
       </c>
-      <c r="I21" s="25">
+      <c r="I19" s="20">
         <f t="shared" si="0"/>
         <v>1.32</v>
       </c>
-      <c r="J21" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="K21" s="19" t="s">
-        <v>80</v>
+      <c r="J19" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="K19" s="11" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="17" t="s">
+        <v>99</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="F20" s="10">
+        <v>1</v>
+      </c>
+      <c r="G20" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="H20" s="10">
+        <v>0.03</v>
+      </c>
+      <c r="I20" s="10">
+        <f t="shared" si="0"/>
+        <v>0.03</v>
+      </c>
+      <c r="J20" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="K20" s="11" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="D21" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="E21" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="F21" s="10">
+        <v>3</v>
+      </c>
+      <c r="G21" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="H21" s="10">
+        <v>0.03</v>
+      </c>
+      <c r="I21" s="10">
+        <f t="shared" si="0"/>
+        <v>0.09</v>
+      </c>
+      <c r="J21" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="K21" s="11" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="G22" s="27" t="s">
-        <v>81</v>
-      </c>
-      <c r="H22" s="27"/>
-      <c r="I22" s="26">
-        <f>SUM(I4:I11)+SUM(I13:I21)</f>
-        <v>22.696000000000002</v>
+      <c r="A22" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="B22" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="D22" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="E22" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="F22" s="10">
+        <v>1</v>
+      </c>
+      <c r="G22" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="H22" s="10">
+        <v>0.03</v>
+      </c>
+      <c r="I22" s="10">
+        <f t="shared" si="0"/>
+        <v>0.03</v>
+      </c>
+      <c r="J22" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="K22" s="11" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="17" t="s">
+        <v>102</v>
+      </c>
+      <c r="B23" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="D23" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="E23" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="F23" s="10">
+        <v>1</v>
+      </c>
+      <c r="G23" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="H23" s="10">
+        <v>0.03</v>
+      </c>
+      <c r="I23" s="10">
+        <f t="shared" si="0"/>
+        <v>0.03</v>
+      </c>
+      <c r="J23" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="K23" s="11" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
+      <c r="A24" s="17" t="s">
+        <v>103</v>
+      </c>
+      <c r="B24" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="F24" s="1">
+      <c r="C24" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="D24" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="E24" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="F24" s="10">
         <v>1</v>
       </c>
+      <c r="G24" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="H24" s="10">
+        <v>0.03</v>
+      </c>
+      <c r="I24" s="10">
+        <f t="shared" si="0"/>
+        <v>0.03</v>
+      </c>
+      <c r="J24" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="K24" s="11" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="F25" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="F26" s="1">
+      <c r="A25" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="B25" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="D25" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="E25" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="F25" s="10">
         <v>1</v>
       </c>
+      <c r="G25" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="H25" s="10">
+        <v>1.58</v>
+      </c>
+      <c r="I25" s="10">
+        <f t="shared" si="0"/>
+        <v>1.58</v>
+      </c>
+      <c r="J25" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="K25" s="11" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="28" t="s">
+        <v>25</v>
+      </c>
+      <c r="B26" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="C26" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="D26" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="E26" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="F26" s="29">
+        <v>1</v>
+      </c>
+      <c r="G26" s="29" t="s">
+        <v>46</v>
+      </c>
+      <c r="H26" s="30">
+        <v>0.45</v>
+      </c>
+      <c r="I26" s="31">
+        <f>H26*F26</f>
+        <v>0.45</v>
+      </c>
+      <c r="J26" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="K26" s="32" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="F27" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="F28" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="F29" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="F30" s="1">
-        <f>SUM(F24:F29)</f>
-        <v>8</v>
+      <c r="G27" s="27" t="s">
+        <v>76</v>
+      </c>
+      <c r="H27" s="27"/>
+      <c r="I27" s="21">
+        <f>SUM(I4:I25)</f>
+        <v>24.806000000000012</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="G27:H27"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="K5" r:id="rId1"/>
@@ -1809,15 +1959,21 @@
     <hyperlink ref="K8" r:id="rId3"/>
     <hyperlink ref="K4" r:id="rId4"/>
     <hyperlink ref="K10" r:id="rId5"/>
-    <hyperlink ref="K20" r:id="rId6"/>
-    <hyperlink ref="K19" r:id="rId7"/>
+    <hyperlink ref="K18" r:id="rId6"/>
+    <hyperlink ref="K17" r:id="rId7"/>
     <hyperlink ref="K11" r:id="rId8"/>
-    <hyperlink ref="K21" r:id="rId9"/>
+    <hyperlink ref="K19" r:id="rId9"/>
+    <hyperlink ref="K20" r:id="rId10"/>
+    <hyperlink ref="K21" r:id="rId11"/>
+    <hyperlink ref="K22" r:id="rId12"/>
+    <hyperlink ref="K23" r:id="rId13"/>
+    <hyperlink ref="K24" r:id="rId14"/>
+    <hyperlink ref="K25" r:id="rId15"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="landscape" horizontalDpi="4294967293" verticalDpi="300" r:id="rId10"/>
+  <pageSetup orientation="landscape" horizontalDpi="4294967293" verticalDpi="300" r:id="rId16"/>
   <ignoredErrors>
-    <ignoredError sqref="G17:G18 G13:G16" numberStoredAsText="1"/>
+    <ignoredError sqref="G16 G12:G15" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Updated to latest files
</commit_message>
<xml_diff>
--- a/BOM/BOM.xlsx
+++ b/BOM/BOM.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="120" windowWidth="19440" windowHeight="9270"/>
@@ -11,7 +11,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
@@ -398,11 +398,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -722,22 +722,22 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -830,7 +830,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -865,7 +864,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1041,14 +1039,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I28" sqref="I28"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="20.85546875" style="1" customWidth="1"/>
     <col min="2" max="2" width="23.5703125" style="1" customWidth="1"/>
@@ -1070,13 +1068,13 @@
     <col min="18" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" ht="15.75" thickBot="1"/>
+    <row r="3" spans="1:11" ht="15.75" thickBot="1">
       <c r="A3" s="13" t="s">
         <v>1</v>
       </c>
@@ -1111,7 +1109,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11">
       <c r="A4" s="22" t="s">
         <v>25</v>
       </c>
@@ -1147,7 +1145,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11">
       <c r="A5" s="5" t="s">
         <v>24</v>
       </c>
@@ -1183,7 +1181,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11">
       <c r="A6" s="5" t="s">
         <v>12</v>
       </c>
@@ -1219,7 +1217,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11">
       <c r="A7" s="5" t="s">
         <v>40</v>
       </c>
@@ -1255,7 +1253,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="8" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" s="9" customFormat="1">
       <c r="A8" s="5" t="s">
         <v>18</v>
       </c>
@@ -1291,7 +1289,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" s="9" customFormat="1">
       <c r="A9" s="5" t="s">
         <v>36</v>
       </c>
@@ -1327,7 +1325,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="10" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" s="9" customFormat="1">
       <c r="A10" s="5" t="s">
         <v>23</v>
       </c>
@@ -1363,7 +1361,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11">
       <c r="A11" s="5" t="s">
         <v>53</v>
       </c>
@@ -1399,7 +1397,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="12" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" s="9" customFormat="1">
       <c r="A12" s="17" t="s">
         <v>78</v>
       </c>
@@ -1435,7 +1433,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" s="9" customFormat="1">
       <c r="A13" s="17" t="s">
         <v>79</v>
       </c>
@@ -1471,7 +1469,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11">
       <c r="A14" s="17" t="s">
         <v>95</v>
       </c>
@@ -1507,7 +1505,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11">
       <c r="A15" s="17" t="s">
         <v>96</v>
       </c>
@@ -1543,7 +1541,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11">
       <c r="A16" s="17" t="s">
         <v>97</v>
       </c>
@@ -1579,7 +1577,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11">
       <c r="A17" s="5" t="s">
         <v>57</v>
       </c>
@@ -1615,7 +1613,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11">
       <c r="A18" s="5" t="s">
         <v>62</v>
       </c>
@@ -1651,7 +1649,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11">
       <c r="A19" s="5" t="s">
         <v>69</v>
       </c>
@@ -1687,7 +1685,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11">
       <c r="A20" s="17" t="s">
         <v>99</v>
       </c>
@@ -1723,7 +1721,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11">
       <c r="A21" s="17" t="s">
         <v>100</v>
       </c>
@@ -1759,7 +1757,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11">
       <c r="A22" s="17" t="s">
         <v>101</v>
       </c>
@@ -1795,7 +1793,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11">
       <c r="A23" s="17" t="s">
         <v>102</v>
       </c>
@@ -1831,7 +1829,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11">
       <c r="A24" s="17" t="s">
         <v>103</v>
       </c>
@@ -1867,7 +1865,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11">
       <c r="A25" s="17" t="s">
         <v>98</v>
       </c>
@@ -1903,47 +1901,47 @@
         <v>119</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="28" t="s">
+    <row r="26" spans="1:11" ht="15.75" thickBot="1">
+      <c r="A26" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="B26" s="29" t="s">
+      <c r="B26" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="C26" s="29" t="s">
+      <c r="C26" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="D26" s="29" t="s">
-        <v>43</v>
-      </c>
-      <c r="E26" s="29" t="s">
+      <c r="D26" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="E26" s="28" t="s">
         <v>45</v>
       </c>
-      <c r="F26" s="29">
+      <c r="F26" s="28">
         <v>1</v>
       </c>
-      <c r="G26" s="29" t="s">
+      <c r="G26" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="H26" s="30">
+      <c r="H26" s="29">
         <v>0.45</v>
       </c>
-      <c r="I26" s="31">
+      <c r="I26" s="30">
         <f>H26*F26</f>
         <v>0.45</v>
       </c>
-      <c r="J26" s="29" t="s">
-        <v>10</v>
-      </c>
-      <c r="K26" s="32" t="s">
+      <c r="J26" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="K26" s="31" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="G27" s="27" t="s">
+    <row r="27" spans="1:11">
+      <c r="G27" s="32" t="s">
         <v>76</v>
       </c>
-      <c r="H27" s="27"/>
+      <c r="H27" s="32"/>
       <c r="I27" s="21">
         <f>SUM(I4:I25)</f>
         <v>24.806000000000012</v>
@@ -1979,24 +1977,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>